<commit_message>
read input from excel
</commit_message>
<xml_diff>
--- a/TravelBuddy/AccomodationExcel.xlsx
+++ b/TravelBuddy/AccomodationExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="191">
   <si>
     <t>Hotel Name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>la 2 km de centru</t>
   </si>
   <si>
-    <t>8,4</t>
-  </si>
-  <si>
     <t>8,2</t>
   </si>
   <si>
@@ -117,487 +114,481 @@
     <t>Ola Living Born</t>
   </si>
   <si>
+    <t>Acta Antibes</t>
+  </si>
+  <si>
+    <t>la 0,8 km de centru</t>
+  </si>
+  <si>
+    <t>Apartment Barcelona Rentals - Park Güell Apartments</t>
+  </si>
+  <si>
+    <t>7,8</t>
+  </si>
+  <si>
+    <t>la 3 km de centru</t>
+  </si>
+  <si>
+    <t>Enjoy Apartments Soho</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>AinB Born-Dames Apartments</t>
+  </si>
+  <si>
+    <t>6,9</t>
+  </si>
+  <si>
+    <t>Classbedroom Born Apartments</t>
+  </si>
+  <si>
+    <t>7,5</t>
+  </si>
+  <si>
+    <t>7,9</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/fridaysflats-5-bedrooms-loft-in-the-heart-of-barcelona.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=15&amp;hapos=590&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=778413101_337665967_11_0_0&amp;highlighted_blocks=778413101_337665967_11_0_0&amp;matching_block_id=778413101_337665967_11_0_0&amp;sr_pri_blocks=778413101_337665967_11_0_0__1460060&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>72.222 lei</t>
+  </si>
+  <si>
+    <t>My Space Barcelona Gracia Pool Terrace</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/gracia-pool-terrace.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=16&amp;hapos=591&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=161717702_326831093_5_0_0%2C161717701_326831093_2_0_0&amp;highlighted_blocks=161717702_326831093_5_0_0%2C161717701_326831093_2_0_0&amp;matching_block_id=161717702_326831093_5_0_0&amp;sr_pri_blocks=161717702_326831093_5_0_0__406200%2C161717701_326831093_2_0_0__269460&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>33.422 lei</t>
+  </si>
+  <si>
+    <t>6,6</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/yate-elmo.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=17&amp;hapos=592&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=41393401_335564999_0_2_0&amp;highlighted_blocks=41393401_335564999_0_2_0&amp;matching_block_id=41393401_335564999_0_2_0&amp;sr_pri_blocks=41393401_335564999_0_2_0__1926968&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>95.318 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/miro-c-barcelona.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=18&amp;hapos=593&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;highlighted_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;matching_block_id=585066302_238409272_2_0_0&amp;sr_pri_blocks=585066302_238409272_2_0_0__253260%2C585066304_238409266_2_0_0__253260%2C585066303_238409266_4_0_0__348720&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>42.305 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/casa-neri.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=19&amp;hapos=594&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;highlighted_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;matching_block_id=637996003_265502871_2_2_0&amp;sr_pri_blocks=637996003_265502871_2_2_0__597335%2C637996001_265502871_3_1_0__694085%2C637996001_265502871_2_2_0__597335&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>93.427 lei</t>
+  </si>
+  <si>
+    <t>AinB Gothic-Jaume I Apartments</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/apartaments-in-barcelona-tiradors.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=20&amp;hapos=595&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0&amp;highlighted_blocks=1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0&amp;matching_block_id=1249906_95135954_2_0_0&amp;sr_pri_blocks=1249906_95135954_2_0_0__280660%2C1249906_95135954_2_0_0__280660%2C1249906_95135954_2_0_0__280660%2C1249906_95135954_2_0_0__280660&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>55.532 lei</t>
+  </si>
+  <si>
+    <t>ClassBedroom Barcelona Beach Apartments</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/barcelona-bedroom.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=21&amp;hapos=596&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1213321_338546902_0_0_0%2C1213322_338546902_0_0_0%2C1213317_338546902_0_0_0%2C1213320_338546902_0_0_0&amp;highlighted_blocks=1213321_338546902_0_0_0%2C1213322_338546902_0_0_0%2C1213317_338546902_0_0_0%2C1213320_338546902_0_0_0&amp;matching_block_id=1213321_338546902_0_0_0&amp;sr_pri_blocks=1213321_338546902_0_0_0__190060%2C1213322_338546902_0_0_0__190060%2C1213317_338546902_0_0_0__190060%2C1213320_338546902_0_0_0__190060&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>37.605 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/ola-living-born.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=22&amp;hapos=597&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=433292203_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;highlighted_blocks=433292203_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;matching_block_id=433292203_221344711_1_0_0&amp;sr_pri_blocks=433292203_221344711_1_0_0__364016%2C433292202_221344711_2_0_0__403276%2C433292202_221344711_2_0_0__403276%2C433292202_221344711_2_0_0__403276&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>77.850 lei</t>
+  </si>
+  <si>
+    <t>Lodging Apartments City Center-Eixample</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/lodging-apartments-sagrada-familia.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=23&amp;hapos=598&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0&amp;highlighted_blocks=68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0&amp;matching_block_id=68967401_298397543_2_0_0&amp;sr_pri_blocks=68967401_298397543_2_0_0__400185%2C68967401_298397543_2_0_0__400185%2C68967401_298397543_2_0_0__400185%2C68967401_298397543_2_0_0__400185&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>79.181 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/apartments-in-barcelona-dames.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=24&amp;hapos=599&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;highlighted_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;matching_block_id=1322401_95137168_2_0_0&amp;sr_pri_blocks=1322401_95137168_2_0_0__245785%2C1322401_95137168_2_0_0__245785%2C1322401_95137168_2_0_0__245785%2C1322401_95137168_2_0_0__245785&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>48.631 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/classbedroom-ii.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=25&amp;hapos=600&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1876407_335854946_2_0_0%2C1876409_335854946_2_0_0%2C1876406_335854946_2_0_0%2C1876408_335854946_2_0_0&amp;highlighted_blocks=1876407_335854946_2_0_0%2C1876409_335854946_2_0_0%2C1876406_335854946_2_0_0%2C1876408_335854946_2_0_0&amp;matching_block_id=1876407_335854946_2_0_0&amp;sr_pri_blocks=1876407_335854946_2_0_0__190840%2C1876409_335854946_2_0_0__190840%2C1876406_335854946_2_0_0__190840%2C1876408_335854946_2_0_0__190840&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>37.760 lei</t>
+  </si>
+  <si>
+    <t>9,5</t>
+  </si>
+  <si>
+    <t>10.716 lei</t>
+  </si>
+  <si>
+    <t>15.303 lei</t>
+  </si>
+  <si>
+    <t>Apartamentos Tarradellas Sants Estació</t>
+  </si>
+  <si>
+    <t>16.604 lei</t>
+  </si>
+  <si>
+    <t>15.509 lei</t>
+  </si>
+  <si>
+    <t>El Alma de las Ramblas</t>
+  </si>
+  <si>
+    <t>32.827 lei</t>
+  </si>
+  <si>
+    <t>Inside Barcelona Apartments Mercat</t>
+  </si>
+  <si>
+    <t>23.237 lei</t>
+  </si>
+  <si>
+    <t>Villa Sagrada</t>
+  </si>
+  <si>
+    <t>18.043 lei</t>
+  </si>
+  <si>
+    <t>18.036 lei</t>
+  </si>
+  <si>
+    <t>44.196 lei</t>
+  </si>
+  <si>
+    <t>60.692 lei</t>
+  </si>
+  <si>
+    <t>61.259 lei</t>
+  </si>
+  <si>
+    <t>42.223 lei</t>
+  </si>
+  <si>
+    <t>Stay U-nique Apartments Vila de Gracia</t>
+  </si>
+  <si>
+    <t>10.954 lei</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>25.852 lei</t>
+  </si>
+  <si>
+    <t>la 0,3 km de centru</t>
+  </si>
+  <si>
+    <t>Stay U-nique Apartments Travessera</t>
+  </si>
+  <si>
+    <t>10.197 lei</t>
+  </si>
+  <si>
+    <t>la 1,9 km de centru</t>
+  </si>
+  <si>
+    <t>26.402 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/quaint-urban-studio-steps-away-from-las-ramblas.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=3&amp;hapos=553&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=576581106_265049109_3_0_0%2C576581104_265049109_3_0_0%2C576581105_265049109_2_0_0&amp;highlighted_blocks=576581106_265049109_3_0_0%2C576581104_265049109_3_0_0%2C576581105_265049109_2_0_0&amp;matching_block_id=576581106_265049109_3_0_0&amp;sr_pri_blocks=576581106_265049109_3_0_0__242240%2C576581104_265049109_3_0_0__242240%2C576581105_265049109_2_0_0__179160&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/inside-bcn-apartments-mercat.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=4&amp;hapos=554&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=28608801_88206329_3_0_0%2C28608802_88206329_2_0_0%2C28608803_88206329_2_0_0&amp;highlighted_blocks=28608801_88206329_3_0_0%2C28608802_88206329_2_0_0%2C28608803_88206329_2_0_0&amp;matching_block_id=28608801_88206329_3_0_0&amp;sr_pri_blocks=28608801_88206329_3_0_0__165840%2C28608802_88206329_2_0_0__135760%2C28608803_88206329_2_0_0__168160&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/bright-family-apartment-with-balcony.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=5&amp;hapos=555&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=723752802_310251050_0_0_0&amp;highlighted_blocks=723752802_310251050_0_0_0&amp;matching_block_id=723752802_310251050_0_0_0&amp;sr_pri_blocks=723752802_310251050_0_0_0__206140&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/villa-sagrada.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=6&amp;hapos=556&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=106837301_175425070_2_0_0%2C106837301_175425070_3_0_0%2C106837301_175425070_2_0_0&amp;highlighted_blocks=106837301_175425070_2_0_0%2C106837301_175425070_3_0_0%2C106837301_175425070_2_0_0&amp;matching_block_id=106837301_175425070_2_0_0&amp;sr_pri_blocks=106837301_175425070_2_0_0__114160%2C106837301_175425070_3_0_0__136440%2C106837301_175425070_2_0_0__114160&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/barcelona-center-tallers.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=7&amp;hapos=557&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=36412101_335678107_2_0_0%2C36412113_88498696_2_0_0%2C36412106_335678107_5_0_0&amp;highlighted_blocks=36412101_335678107_2_0_0%2C36412113_88498696_2_0_0%2C36412106_335678107_5_0_0&amp;matching_block_id=36412101_335678107_2_0_0&amp;sr_pri_blocks=36412101_335678107_2_0_0__142024%2C36412113_88498696_2_0_0__164260%2C36412106_335678107_5_0_0__227458&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/global-apartments.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=8&amp;hapos=558&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=710970401_295953354_2_0_1099511627776%2C710970404_295953354_0_0_0%2C710970404_295953354_0_0_0&amp;highlighted_blocks=710970401_295953354_2_0_1099511627776%2C710970404_295953354_0_0_0%2C710970404_295953354_0_0_0&amp;matching_block_id=710970401_295953354_2_0_1099511627776&amp;sr_pri_blocks=710970401_295953354_2_0_1099511627776__157242%2C710970404_295953354_0_0_0__103694%2C710970404_295953354_0_0_0__103694&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/fridaysflats-5-bedrooms-loft-in-the-heart-of-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=9&amp;hapos=559&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=778413101_337665967_11_0_0&amp;highlighted_blocks=778413101_337665967_11_0_0&amp;matching_block_id=778413101_337665967_11_0_0&amp;sr_pri_blocks=778413101_337665967_11_0_0__893480&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/yate-elmo.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=10&amp;hapos=560&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=41393401_335564999_0_2_0&amp;highlighted_blocks=41393401_335564999_0_2_0&amp;matching_block_id=41393401_335564999_0_2_0&amp;sr_pri_blocks=41393401_335564999_0_2_0__1226968&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/charming-apartment-in-gracia-with-a-sunny-balcony.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=11&amp;hapos=561&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=739112405_328588968_8_0_0&amp;highlighted_blocks=739112405_328588968_8_0_0&amp;matching_block_id=739112405_328588968_8_0_0&amp;sr_pri_blocks=739112405_328588968_8_0_0__221440&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/miro-c-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=12&amp;hapos=562&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;highlighted_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;matching_block_id=585066302_238409272_2_0_0&amp;sr_pri_blocks=585066302_238409272_2_0_0__155360%2C585066304_238409266_2_0_0__155360%2C585066303_238409266_4_0_0__211920&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/casa-neri.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=13&amp;hapos=563&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;highlighted_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;matching_block_id=637996003_265502871_2_2_0&amp;sr_pri_blocks=637996003_265502871_2_2_0__392060%2C637996001_265502871_3_1_0__454300%2C637996001_265502871_2_2_0__392060&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/ola-living-born.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=14&amp;hapos=564&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=433292202_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;highlighted_blocks=433292202_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;matching_block_id=433292202_221344711_1_0_0&amp;sr_pri_blocks=433292202_221344711_1_0_0__201368%2C433292202_221344711_2_0_0__217408%2C433292202_221344711_2_0_0__217408%2C433292202_221344711_2_0_0__217408&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/esparteria-2.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=11&amp;hapos=11&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=798650501_340215862_8_0_0&amp;highlighted_blocks=798650501_340215862_8_0_0&amp;matching_block_id=798650501_340215862_8_0_0&amp;sr_pri_blocks=798650501_340215862_8_0_0__216640&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>Alcam Calabria</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/alcam-calabria.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=12&amp;hapos=12&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=267478101_105800329_0_0_0&amp;highlighted_blocks=267478101_105800329_0_0_0&amp;matching_block_id=267478101_105800329_0_0_0&amp;sr_pri_blocks=267478101_105800329_0_0_0__179440&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>8.876 lei</t>
+  </si>
+  <si>
+    <t>la 1,5 km de centru</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/amplio-y-bien-situado-para-10-personas.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=13&amp;hapos=13&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=77877103_326137462_0_0_0&amp;highlighted_blocks=77877103_326137462_0_0_0&amp;matching_block_id=77877103_326137462_0_0_0&amp;sr_pri_blocks=77877103_326137462_0_0_0__335680&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/apartment-barcelona-rentals-duplex-apartments-near-park-guell.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=14&amp;hapos=14&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=188370102_295479163_8_0_0&amp;highlighted_blocks=188370102_295479163_8_0_0&amp;matching_block_id=188370102_295479163_8_0_0&amp;sr_pri_blocks=188370102_295479163_8_0_0__313540&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>New!Charming appartement in the heart of Barcelona</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/new-charming-appartement-in-the-heart-of-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=15&amp;hapos=15&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=770432101_334870003_5_0_6047313952768&amp;highlighted_blocks=770432101_334870003_5_0_6047313952768&amp;matching_block_id=770432101_334870003_5_0_6047313952768&amp;sr_pri_blocks=770432101_334870003_5_0_6047313952768__270100&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>13.361 lei</t>
+  </si>
+  <si>
+    <t>9,7</t>
+  </si>
+  <si>
+    <t>Eurohotel Diagonal Port</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/rafaeldiagonal.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=16&amp;hapos=16&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=9029209_239874675_4_0_0%2C9029210_239874675_2_0_0%2C9029210_239874675_2_0_0&amp;highlighted_blocks=9029209_239874675_4_0_0%2C9029210_239874675_2_0_0%2C9029210_239874675_2_0_0&amp;matching_block_id=9029209_239874675_4_0_0&amp;sr_pri_blocks=9029209_239874675_4_0_0__158940%2C9029210_239874675_2_0_0__96020%2C9029210_239874675_2_0_0__96020&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>17.361 lei</t>
+  </si>
+  <si>
+    <t>la 3,6 km de centru</t>
+  </si>
+  <si>
+    <t>VINTAGE - Plaza Universidad</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/vintage-plaza-universidad-5bedrooms-47-2bathrooms.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=17&amp;hapos=17&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=211903802_310243829_5_0_6047313952768&amp;highlighted_blocks=211903802_310243829_5_0_6047313952768&amp;matching_block_id=211903802_310243829_5_0_6047313952768&amp;sr_pri_blocks=211903802_310243829_5_0_6047313952768__273700&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>13.539 lei</t>
+  </si>
+  <si>
+    <t>6 dormitorios en Apartamento Modernista en el Corazon de Barcelona</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/6-dormitorios-en-apartamento-modernista-en-el-corazon-de-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=18&amp;hapos=18&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=636402601_326659653_12_0_0&amp;highlighted_blocks=636402601_326659653_12_0_0&amp;matching_block_id=636402601_326659653_12_0_0&amp;sr_pri_blocks=636402601_326659653_12_0_0__630160&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>31.171 lei</t>
+  </si>
+  <si>
+    <t>la 300 m de centru</t>
+  </si>
+  <si>
+    <t>Stay U-nique Apartments Roger Llúria II</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/stay-u-nique-roger-de-lluria-ii.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=19&amp;hapos=19&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=598003301_234383729_0_0_0&amp;highlighted_blocks=598003301_234383729_0_0_0&amp;matching_block_id=598003301_234383729_0_0_0&amp;sr_pri_blocks=598003301_234383729_0_0_0__260440&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>12.883 lei</t>
+  </si>
+  <si>
+    <t>Ilunion Auditori</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/confortel-auditori.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=20&amp;hapos=20&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=9277410_107323228_0_2_0%2C9277410_107323228_0_2_0%2C9277401_107323228_0_2_0&amp;highlighted_blocks=9277410_107323228_0_2_0%2C9277410_107323228_0_2_0%2C9277401_107323228_0_2_0&amp;matching_block_id=9277410_107323228_0_2_0&amp;sr_pri_blocks=9277410_107323228_0_2_0__151182%2C9277410_107323228_0_2_0__151182%2C9277401_107323228_0_2_0__135342&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>21.651 lei</t>
+  </si>
+  <si>
+    <t>Duplex Sagrada Familia</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/duplex-sagrada-familia.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=21&amp;hapos=21&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=467147602_333927248_0_0_0&amp;highlighted_blocks=467147602_333927248_0_0_0&amp;matching_block_id=467147602_333927248_0_0_0&amp;sr_pri_blocks=467147602_333927248_0_0_0__223780&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>11.069 lei</t>
+  </si>
+  <si>
+    <t>8,1</t>
+  </si>
+  <si>
+    <t>Hostal Portugal</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/pension-portugal.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=22&amp;hapos=22&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=27524208_88206095_0_0_0%2C27524208_88206095_0_0_0%2C27524205_88206095_0_0_0&amp;highlighted_blocks=27524208_88206095_0_0_0%2C27524208_88206095_0_0_0%2C27524205_88206095_0_0_0&amp;matching_block_id=27524208_88206095_0_0_0&amp;sr_pri_blocks=27524208_88206095_0_0_0__42042%2C27524208_88206095_0_0_0__42042%2C27524205_88206095_0_0_0__42042&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>6.239 lei</t>
+  </si>
+  <si>
+    <t>Unique Cozy Scenic Penthouse</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/unique-cozy-scenic-penthouse.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=23&amp;hapos=23&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=198952601_119720213_7_0_0&amp;highlighted_blocks=198952601_119720213_7_0_0&amp;matching_block_id=198952601_119720213_7_0_0&amp;sr_pri_blocks=198952601_119720213_7_0_0__298560&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>14.768 lei</t>
+  </si>
+  <si>
+    <t>la 2,5 km de centru</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/hotelantibesbarcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=24&amp;hapos=24&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=9131901_246265787_0_2_0%2C9131903_246265787_0_2_0%2C9131903_246265787_0_2_0&amp;highlighted_blocks=9131901_246265787_0_2_0%2C9131903_246265787_0_2_0%2C9131903_246265787_0_2_0&amp;matching_block_id=9131901_246265787_0_2_0&amp;sr_pri_blocks=9131901_246265787_0_2_0__81192%2C9131903_246265787_0_2_0__114093%2C9131903_246265787_0_2_0__114093&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>Casa Gracia</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/hostel-casa-gracia.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=25&amp;hapos=25&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=25515426_295384839_0_0_0%2C25515426_295384839_0_0_0&amp;highlighted_blocks=25515426_295384839_0_0_0%2C25515426_295384839_0_0_0&amp;matching_block_id=25515426_295384839_0_0_0&amp;sr_pri_blocks=25515426_295384839_0_0_0__176184%2C25515426_295384839_0_0_0__176184&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>17.430 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/apartments-in-barcelona-dames.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=1&amp;hapos=651&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506110&amp;all_sr_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;highlighted_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;matching_block_id=1322401_95137168_2_0_0&amp;sr_pri_blocks=1322401_95137168_2_0_0__144535%2C1322401_95137168_2_0_0__144535%2C1322401_95137168_2_0_0__144535%2C1322401_95137168_2_0_0__144535&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>28.598 lei</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/classbedroom-ii.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=2&amp;hapos=652&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506110&amp;all_sr_blocks=1876408_335854946_2_0_0%2C1876407_335854946_2_0_0%2C1876405_335854946_2_0_0%2C1876406_335854946_2_0_0&amp;highlighted_blocks=1876408_335854946_2_0_0%2C1876407_335854946_2_0_0%2C1876405_335854946_2_0_0%2C1876406_335854946_2_0_0&amp;matching_block_id=1876408_335854946_2_0_0&amp;sr_pri_blocks=1876408_335854946_2_0_0__105700%2C1876407_335854946_2_0_0__105700%2C1876405_335854946_2_0_0__105700%2C1876406_335854946_2_0_0__105700&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>20.914 lei</t>
+  </si>
+  <si>
+    <t>Signature Apartments Diagonal</t>
+  </si>
+  <si>
+    <t>14.490 lei</t>
+  </si>
+  <si>
+    <t>la 1,8 km de centru</t>
+  </si>
+  <si>
+    <t>Anima Apartments Sants</t>
+  </si>
+  <si>
+    <t>9.525 lei</t>
+  </si>
+  <si>
+    <t>la 3,5 km de centru</t>
+  </si>
+  <si>
+    <t>Apartments Barcelona &amp; Home Deco Centro</t>
+  </si>
+  <si>
+    <t>22.446 lei</t>
+  </si>
+  <si>
+    <t>la 200 m de centru</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/signature-apartments-diagonal-aribau.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=1&amp;hapos=1&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=624402004_247208445_7_0_0&amp;highlighted_blocks=624402004_247208445_7_0_0&amp;matching_block_id=624402004_247208445_7_0_0&amp;sr_pri_blocks=624402004_247208445_7_0_0__293060&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/animapartments-sants.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=2&amp;hapos=2&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=319066107_341731389_8_0_0&amp;highlighted_blocks=319066107_341731389_8_0_0&amp;matching_block_id=319066107_341731389_8_0_0&amp;sr_pri_blocks=319066107_341731389_8_0_0__192640&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/apartments-barcelona-amp-home-deco-centro.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=3&amp;hapos=3&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=73721302_325509721_7_0_0&amp;highlighted_blocks=73721302_325509721_7_0_0&amp;matching_block_id=73721302_325509721_7_0_0&amp;sr_pri_blocks=73721302_325509721_7_0_0__453960&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>Cal Mateu</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/ca-39-l-mateu.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=4&amp;hapos=4&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=240710701_178269580_0_0_0&amp;highlighted_blocks=240710701_178269580_0_0_0&amp;matching_block_id=240710701_178269580_0_0_0&amp;sr_pri_blocks=240710701_178269580_0_0_0__317640&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>15.706 lei</t>
+  </si>
+  <si>
+    <t>Hotel Peninsular</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/peninsular-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=5&amp;hapos=5&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=38860901_266040762_0_1_0%2C38860902_266040762_0_1_0%2C38860903_266040762_0_1_0&amp;highlighted_blocks=38860901_266040762_0_1_0%2C38860902_266040762_0_1_0%2C38860903_266040762_0_1_0&amp;matching_block_id=38860901_266040762_0_1_0&amp;sr_pri_blocks=38860901_266040762_0_1_0__62121%2C38860902_266040762_0_1_0__93042%2C38860903_266040762_0_1_0__120363&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>13.623 lei</t>
+  </si>
+  <si>
+    <t>la 0,9 km de centru</t>
+  </si>
+  <si>
+    <t>BCN Urbaness Hotels Del Comte</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/delcomte.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=6&amp;hapos=6&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=9106016_335554454_2_2_0%2C9106008_335554454_0_2_0%2C9106008_335554454_0_2_0&amp;highlighted_blocks=9106016_335554454_2_2_0%2C9106008_335554454_0_2_0%2C9106008_335554454_0_2_0&amp;matching_block_id=9106016_335554454_2_2_0&amp;sr_pri_blocks=9106016_335554454_2_2_0__82527%2C9106008_335554454_0_2_0__110148%2C9106008_335554454_0_2_0__110148&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>14.973 lei</t>
+  </si>
+  <si>
+    <t>Bcn Paseo De Gracia Rocamora Apartment</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/bcn-paseo-de-gracia-aparment.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=7&amp;hapos=7&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=73058510_338023110_0_0_0&amp;highlighted_blocks=73058510_338023110_0_0_0&amp;matching_block_id=73058510_338023110_0_0_0&amp;sr_pri_blocks=73058510_338023110_0_0_0__415560&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>20.547 lei</t>
+  </si>
+  <si>
+    <t>Victoria Diagonal Mar Barcelona</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/victoria-diagonal-mar-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=8&amp;hapos=8&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=130345401_340824879_6_0_0&amp;highlighted_blocks=130345401_340824879_6_0_0&amp;matching_block_id=130345401_340824879_6_0_0&amp;sr_pri_blocks=130345401_340824879_6_0_0__368780&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>18.234 lei</t>
+  </si>
+  <si>
+    <t>la 3,7 km de centru</t>
+  </si>
+  <si>
+    <t>Hostalin Barcelona Diputación</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/hotel/es/hostalin-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=9&amp;hapos=9&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=39007205_298407854_0_0_0%2C39007205_298407854_0_0_0%2C39007205_298407854_0_0_0&amp;highlighted_blocks=39007205_298407854_0_0_0%2C39007205_298407854_0_0_0%2C39007205_298407854_0_0_0&amp;matching_block_id=39007205_298407854_0_0_0&amp;sr_pri_blocks=39007205_298407854_0_0_0__60942%2C39007205_298407854_0_0_0__60942%2C39007205_298407854_0_0_0__60942&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>9.040 lei</t>
+  </si>
+  <si>
     <t>7,2</t>
   </si>
   <si>
-    <t>Acta Antibes</t>
-  </si>
-  <si>
-    <t>la 3,2 km de centru</t>
-  </si>
-  <si>
-    <t>la 0,8 km de centru</t>
-  </si>
-  <si>
-    <t>Sallés Hotel Pere IV</t>
-  </si>
-  <si>
-    <t>la 2,2 km de centru</t>
-  </si>
-  <si>
-    <t>Apartment Guell</t>
-  </si>
-  <si>
-    <t>9,4</t>
-  </si>
-  <si>
-    <t>Apartment Barcelona Rentals - Park Güell Apartments</t>
-  </si>
-  <si>
-    <t>7,8</t>
-  </si>
-  <si>
-    <t>la 3 km de centru</t>
-  </si>
-  <si>
-    <t>Enjoy Apartments Soho</t>
-  </si>
-  <si>
-    <t>7,7</t>
-  </si>
-  <si>
-    <t>AinB Born-Dames Apartments</t>
-  </si>
-  <si>
-    <t>6,9</t>
-  </si>
-  <si>
-    <t>Classbedroom Born Apartments</t>
-  </si>
-  <si>
-    <t>Hotel Peninsular</t>
-  </si>
-  <si>
-    <t>7,5</t>
-  </si>
-  <si>
-    <t>la 0,9 km de centru</t>
-  </si>
-  <si>
-    <t>7,9</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/fridaysflats-5-bedrooms-loft-in-the-heart-of-barcelona.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=15&amp;hapos=590&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=778413101_337665967_11_0_0&amp;highlighted_blocks=778413101_337665967_11_0_0&amp;matching_block_id=778413101_337665967_11_0_0&amp;sr_pri_blocks=778413101_337665967_11_0_0__1460060&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>72.222 lei</t>
-  </si>
-  <si>
-    <t>My Space Barcelona Gracia Pool Terrace</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/gracia-pool-terrace.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=16&amp;hapos=591&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=161717702_326831093_5_0_0%2C161717701_326831093_2_0_0&amp;highlighted_blocks=161717702_326831093_5_0_0%2C161717701_326831093_2_0_0&amp;matching_block_id=161717702_326831093_5_0_0&amp;sr_pri_blocks=161717702_326831093_5_0_0__406200%2C161717701_326831093_2_0_0__269460&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>33.422 lei</t>
-  </si>
-  <si>
-    <t>6,6</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/yate-elmo.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=17&amp;hapos=592&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=41393401_335564999_0_2_0&amp;highlighted_blocks=41393401_335564999_0_2_0&amp;matching_block_id=41393401_335564999_0_2_0&amp;sr_pri_blocks=41393401_335564999_0_2_0__1926968&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>95.318 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/miro-c-barcelona.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=18&amp;hapos=593&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;highlighted_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;matching_block_id=585066302_238409272_2_0_0&amp;sr_pri_blocks=585066302_238409272_2_0_0__253260%2C585066304_238409266_2_0_0__253260%2C585066303_238409266_4_0_0__348720&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>42.305 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/casa-neri.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=19&amp;hapos=594&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;highlighted_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;matching_block_id=637996003_265502871_2_2_0&amp;sr_pri_blocks=637996003_265502871_2_2_0__597335%2C637996001_265502871_3_1_0__694085%2C637996001_265502871_2_2_0__597335&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>93.427 lei</t>
-  </si>
-  <si>
-    <t>AinB Gothic-Jaume I Apartments</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/apartaments-in-barcelona-tiradors.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=20&amp;hapos=595&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0&amp;highlighted_blocks=1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0%2C1249906_95135954_2_0_0&amp;matching_block_id=1249906_95135954_2_0_0&amp;sr_pri_blocks=1249906_95135954_2_0_0__280660%2C1249906_95135954_2_0_0__280660%2C1249906_95135954_2_0_0__280660%2C1249906_95135954_2_0_0__280660&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>55.532 lei</t>
-  </si>
-  <si>
-    <t>ClassBedroom Barcelona Beach Apartments</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/barcelona-bedroom.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=21&amp;hapos=596&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1213321_338546902_0_0_0%2C1213322_338546902_0_0_0%2C1213317_338546902_0_0_0%2C1213320_338546902_0_0_0&amp;highlighted_blocks=1213321_338546902_0_0_0%2C1213322_338546902_0_0_0%2C1213317_338546902_0_0_0%2C1213320_338546902_0_0_0&amp;matching_block_id=1213321_338546902_0_0_0&amp;sr_pri_blocks=1213321_338546902_0_0_0__190060%2C1213322_338546902_0_0_0__190060%2C1213317_338546902_0_0_0__190060%2C1213320_338546902_0_0_0__190060&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>37.605 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/ola-living-born.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=22&amp;hapos=597&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=433292203_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;highlighted_blocks=433292203_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;matching_block_id=433292203_221344711_1_0_0&amp;sr_pri_blocks=433292203_221344711_1_0_0__364016%2C433292202_221344711_2_0_0__403276%2C433292202_221344711_2_0_0__403276%2C433292202_221344711_2_0_0__403276&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>77.850 lei</t>
-  </si>
-  <si>
-    <t>Lodging Apartments City Center-Eixample</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/lodging-apartments-sagrada-familia.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=23&amp;hapos=598&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0&amp;highlighted_blocks=68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0%2C68967401_298397543_2_0_0&amp;matching_block_id=68967401_298397543_2_0_0&amp;sr_pri_blocks=68967401_298397543_2_0_0__400185%2C68967401_298397543_2_0_0__400185%2C68967401_298397543_2_0_0__400185%2C68967401_298397543_2_0_0__400185&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>79.181 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/apartments-in-barcelona-dames.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=24&amp;hapos=599&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;highlighted_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;matching_block_id=1322401_95137168_2_0_0&amp;sr_pri_blocks=1322401_95137168_2_0_0__245785%2C1322401_95137168_2_0_0__245785%2C1322401_95137168_2_0_0__245785%2C1322401_95137168_2_0_0__245785&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>48.631 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/classbedroom-ii.ro.html?label=gen173nr-1DCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AED6AEBiAIBqAIDuAL_nN2OBsACAdICJDhmYTliYjA4LWEzZWYtNGE3NS1hZDYzLWFkMDZmMDgyZGM1YtgCBOACAQ&amp;sid=859788d0358ebf90d6571f773143c0c2&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-12-10&amp;checkout=2022-12-29&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=25&amp;hapos=600&amp;sr_order=popularity&amp;srpvid=247a8ede8f52016b&amp;srepoch=1641500395&amp;all_sr_blocks=1876407_335854946_2_0_0%2C1876409_335854946_2_0_0%2C1876406_335854946_2_0_0%2C1876408_335854946_2_0_0&amp;highlighted_blocks=1876407_335854946_2_0_0%2C1876409_335854946_2_0_0%2C1876406_335854946_2_0_0%2C1876408_335854946_2_0_0&amp;matching_block_id=1876407_335854946_2_0_0&amp;sr_pri_blocks=1876407_335854946_2_0_0__190840%2C1876409_335854946_2_0_0__190840%2C1876406_335854946_2_0_0__190840%2C1876408_335854946_2_0_0__190840&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>37.760 lei</t>
-  </si>
-  <si>
-    <t>9,5</t>
-  </si>
-  <si>
-    <t>13.629 lei</t>
-  </si>
-  <si>
-    <t>Hostalin Barcelona Diputación</t>
-  </si>
-  <si>
-    <t>9.044 lei</t>
-  </si>
-  <si>
-    <t>19.163 lei</t>
-  </si>
-  <si>
-    <t>Sagrada Familia Apartment</t>
-  </si>
-  <si>
-    <t>9.847 lei</t>
-  </si>
-  <si>
-    <t>12.423 lei</t>
-  </si>
-  <si>
-    <t>10.716 lei</t>
-  </si>
-  <si>
-    <t>15.303 lei</t>
-  </si>
-  <si>
-    <t>Apartamentos Tarradellas Sants Estació</t>
-  </si>
-  <si>
-    <t>16.604 lei</t>
-  </si>
-  <si>
-    <t>15.509 lei</t>
-  </si>
-  <si>
-    <t>El Alma de las Ramblas</t>
-  </si>
-  <si>
-    <t>32.827 lei</t>
-  </si>
-  <si>
-    <t>Inside Barcelona Apartments Mercat</t>
-  </si>
-  <si>
-    <t>23.237 lei</t>
-  </si>
-  <si>
-    <t>Villa Sagrada</t>
-  </si>
-  <si>
-    <t>18.043 lei</t>
-  </si>
-  <si>
-    <t>18.036 lei</t>
-  </si>
-  <si>
-    <t>44.196 lei</t>
-  </si>
-  <si>
-    <t>60.692 lei</t>
-  </si>
-  <si>
-    <t>61.259 lei</t>
-  </si>
-  <si>
-    <t>42.223 lei</t>
-  </si>
-  <si>
-    <t>Cal Mateu</t>
-  </si>
-  <si>
-    <t>15.712 lei</t>
-  </si>
-  <si>
-    <t>Hostal Orleans</t>
-  </si>
-  <si>
-    <t>16.918 lei</t>
-  </si>
-  <si>
-    <t>Stay U-nique Apartments Vila de Gracia</t>
-  </si>
-  <si>
-    <t>10.954 lei</t>
-  </si>
-  <si>
-    <t>5,3</t>
-  </si>
-  <si>
-    <t>25.852 lei</t>
-  </si>
-  <si>
-    <t>la 0,3 km de centru</t>
-  </si>
-  <si>
-    <t>Stay U-nique Apartments Travessera</t>
-  </si>
-  <si>
-    <t>10.197 lei</t>
-  </si>
-  <si>
-    <t>la 1,9 km de centru</t>
-  </si>
-  <si>
-    <t>26.402 lei</t>
-  </si>
-  <si>
-    <t>Luxury UPC-Forum-CCIB-Apart ment</t>
-  </si>
-  <si>
-    <t>15.109 lei</t>
-  </si>
-  <si>
-    <t>la 5,5 km de centru</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/quaint-urban-studio-steps-away-from-las-ramblas.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=3&amp;hapos=553&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=576581106_265049109_3_0_0%2C576581104_265049109_3_0_0%2C576581105_265049109_2_0_0&amp;highlighted_blocks=576581106_265049109_3_0_0%2C576581104_265049109_3_0_0%2C576581105_265049109_2_0_0&amp;matching_block_id=576581106_265049109_3_0_0&amp;sr_pri_blocks=576581106_265049109_3_0_0__242240%2C576581104_265049109_3_0_0__242240%2C576581105_265049109_2_0_0__179160&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/inside-bcn-apartments-mercat.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=4&amp;hapos=554&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=28608801_88206329_3_0_0%2C28608802_88206329_2_0_0%2C28608803_88206329_2_0_0&amp;highlighted_blocks=28608801_88206329_3_0_0%2C28608802_88206329_2_0_0%2C28608803_88206329_2_0_0&amp;matching_block_id=28608801_88206329_3_0_0&amp;sr_pri_blocks=28608801_88206329_3_0_0__165840%2C28608802_88206329_2_0_0__135760%2C28608803_88206329_2_0_0__168160&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/bright-family-apartment-with-balcony.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=5&amp;hapos=555&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=723752802_310251050_0_0_0&amp;highlighted_blocks=723752802_310251050_0_0_0&amp;matching_block_id=723752802_310251050_0_0_0&amp;sr_pri_blocks=723752802_310251050_0_0_0__206140&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/villa-sagrada.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=6&amp;hapos=556&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=106837301_175425070_2_0_0%2C106837301_175425070_3_0_0%2C106837301_175425070_2_0_0&amp;highlighted_blocks=106837301_175425070_2_0_0%2C106837301_175425070_3_0_0%2C106837301_175425070_2_0_0&amp;matching_block_id=106837301_175425070_2_0_0&amp;sr_pri_blocks=106837301_175425070_2_0_0__114160%2C106837301_175425070_3_0_0__136440%2C106837301_175425070_2_0_0__114160&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/barcelona-center-tallers.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=7&amp;hapos=557&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=36412101_335678107_2_0_0%2C36412113_88498696_2_0_0%2C36412106_335678107_5_0_0&amp;highlighted_blocks=36412101_335678107_2_0_0%2C36412113_88498696_2_0_0%2C36412106_335678107_5_0_0&amp;matching_block_id=36412101_335678107_2_0_0&amp;sr_pri_blocks=36412101_335678107_2_0_0__142024%2C36412113_88498696_2_0_0__164260%2C36412106_335678107_5_0_0__227458&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/global-apartments.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=8&amp;hapos=558&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=710970401_295953354_2_0_1099511627776%2C710970404_295953354_0_0_0%2C710970404_295953354_0_0_0&amp;highlighted_blocks=710970401_295953354_2_0_1099511627776%2C710970404_295953354_0_0_0%2C710970404_295953354_0_0_0&amp;matching_block_id=710970401_295953354_2_0_1099511627776&amp;sr_pri_blocks=710970401_295953354_2_0_1099511627776__157242%2C710970404_295953354_0_0_0__103694%2C710970404_295953354_0_0_0__103694&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/fridaysflats-5-bedrooms-loft-in-the-heart-of-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=9&amp;hapos=559&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=778413101_337665967_11_0_0&amp;highlighted_blocks=778413101_337665967_11_0_0&amp;matching_block_id=778413101_337665967_11_0_0&amp;sr_pri_blocks=778413101_337665967_11_0_0__893480&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/yate-elmo.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=10&amp;hapos=560&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=41393401_335564999_0_2_0&amp;highlighted_blocks=41393401_335564999_0_2_0&amp;matching_block_id=41393401_335564999_0_2_0&amp;sr_pri_blocks=41393401_335564999_0_2_0__1226968&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/charming-apartment-in-gracia-with-a-sunny-balcony.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=11&amp;hapos=561&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=739112405_328588968_8_0_0&amp;highlighted_blocks=739112405_328588968_8_0_0&amp;matching_block_id=739112405_328588968_8_0_0&amp;sr_pri_blocks=739112405_328588968_8_0_0__221440&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/miro-c-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=12&amp;hapos=562&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;highlighted_blocks=585066302_238409272_2_0_0%2C585066304_238409266_2_0_0%2C585066303_238409266_4_0_0&amp;matching_block_id=585066302_238409272_2_0_0&amp;sr_pri_blocks=585066302_238409272_2_0_0__155360%2C585066304_238409266_2_0_0__155360%2C585066303_238409266_4_0_0__211920&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/casa-neri.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=13&amp;hapos=563&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;highlighted_blocks=637996003_265502871_2_2_0%2C637996001_265502871_3_1_0%2C637996001_265502871_2_2_0&amp;matching_block_id=637996003_265502871_2_2_0&amp;sr_pri_blocks=637996003_265502871_2_2_0__392060%2C637996001_265502871_3_1_0__454300%2C637996001_265502871_2_2_0__392060&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/ola-living-born.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAKLwt2OBsACAdICJDYzOTljZTc4LThjZjAtNGE3NC05YTRiLTQyNjMxZTRiZTc2NdgCBuACAQ&amp;sid=58e21baa4655679d71f9f487db6add0e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=14&amp;hapos=564&amp;sr_order=popularity&amp;srpvid=3a88982ce68b021f&amp;srepoch=1641505153&amp;all_sr_blocks=433292202_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;highlighted_blocks=433292202_221344711_1_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0%2C433292202_221344711_2_0_0&amp;matching_block_id=433292202_221344711_1_0_0&amp;sr_pri_blocks=433292202_221344711_1_0_0__201368%2C433292202_221344711_2_0_0__217408%2C433292202_221344711_2_0_0__217408%2C433292202_221344711_2_0_0__217408&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>Fridays Flats Casa Flor, Villa with Pool</t>
-  </si>
-  <si>
-    <t>23.523 lei</t>
-  </si>
-  <si>
-    <t>la 4,3 km de centru</t>
-  </si>
-  <si>
-    <t>Stay U-nique Apartments Girona</t>
-  </si>
-  <si>
-    <t>11.498 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/esparteria-2.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=11&amp;hapos=11&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=798650501_340215862_8_0_0&amp;highlighted_blocks=798650501_340215862_8_0_0&amp;matching_block_id=798650501_340215862_8_0_0&amp;sr_pri_blocks=798650501_340215862_8_0_0__216640&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>Alcam Calabria</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/alcam-calabria.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=12&amp;hapos=12&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=267478101_105800329_0_0_0&amp;highlighted_blocks=267478101_105800329_0_0_0&amp;matching_block_id=267478101_105800329_0_0_0&amp;sr_pri_blocks=267478101_105800329_0_0_0__179440&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>8.876 lei</t>
-  </si>
-  <si>
-    <t>la 1,5 km de centru</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/amplio-y-bien-situado-para-10-personas.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=13&amp;hapos=13&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=77877103_326137462_0_0_0&amp;highlighted_blocks=77877103_326137462_0_0_0&amp;matching_block_id=77877103_326137462_0_0_0&amp;sr_pri_blocks=77877103_326137462_0_0_0__335680&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/apartment-barcelona-rentals-duplex-apartments-near-park-guell.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=14&amp;hapos=14&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=188370102_295479163_8_0_0&amp;highlighted_blocks=188370102_295479163_8_0_0&amp;matching_block_id=188370102_295479163_8_0_0&amp;sr_pri_blocks=188370102_295479163_8_0_0__313540&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>New!Charming appartement in the heart of Barcelona</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/new-charming-appartement-in-the-heart-of-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=15&amp;hapos=15&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=770432101_334870003_5_0_6047313952768&amp;highlighted_blocks=770432101_334870003_5_0_6047313952768&amp;matching_block_id=770432101_334870003_5_0_6047313952768&amp;sr_pri_blocks=770432101_334870003_5_0_6047313952768__270100&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>13.361 lei</t>
-  </si>
-  <si>
-    <t>9,7</t>
-  </si>
-  <si>
-    <t>Eurohotel Diagonal Port</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/rafaeldiagonal.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=16&amp;hapos=16&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=9029209_239874675_4_0_0%2C9029210_239874675_2_0_0%2C9029210_239874675_2_0_0&amp;highlighted_blocks=9029209_239874675_4_0_0%2C9029210_239874675_2_0_0%2C9029210_239874675_2_0_0&amp;matching_block_id=9029209_239874675_4_0_0&amp;sr_pri_blocks=9029209_239874675_4_0_0__158940%2C9029210_239874675_2_0_0__96020%2C9029210_239874675_2_0_0__96020&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>17.361 lei</t>
-  </si>
-  <si>
-    <t>la 3,6 km de centru</t>
-  </si>
-  <si>
-    <t>VINTAGE - Plaza Universidad</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/vintage-plaza-universidad-5bedrooms-47-2bathrooms.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=17&amp;hapos=17&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=211903802_310243829_5_0_6047313952768&amp;highlighted_blocks=211903802_310243829_5_0_6047313952768&amp;matching_block_id=211903802_310243829_5_0_6047313952768&amp;sr_pri_blocks=211903802_310243829_5_0_6047313952768__273700&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>13.539 lei</t>
-  </si>
-  <si>
-    <t>6 dormitorios en Apartamento Modernista en el Corazon de Barcelona</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/6-dormitorios-en-apartamento-modernista-en-el-corazon-de-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=18&amp;hapos=18&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=636402601_326659653_12_0_0&amp;highlighted_blocks=636402601_326659653_12_0_0&amp;matching_block_id=636402601_326659653_12_0_0&amp;sr_pri_blocks=636402601_326659653_12_0_0__630160&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>31.171 lei</t>
-  </si>
-  <si>
-    <t>la 300 m de centru</t>
-  </si>
-  <si>
-    <t>Stay U-nique Apartments Roger Llúria II</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/stay-u-nique-roger-de-lluria-ii.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=19&amp;hapos=19&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=598003301_234383729_0_0_0&amp;highlighted_blocks=598003301_234383729_0_0_0&amp;matching_block_id=598003301_234383729_0_0_0&amp;sr_pri_blocks=598003301_234383729_0_0_0__260440&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>12.883 lei</t>
-  </si>
-  <si>
-    <t>Ilunion Auditori</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/confortel-auditori.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=20&amp;hapos=20&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=9277410_107323228_0_2_0%2C9277410_107323228_0_2_0%2C9277401_107323228_0_2_0&amp;highlighted_blocks=9277410_107323228_0_2_0%2C9277410_107323228_0_2_0%2C9277401_107323228_0_2_0&amp;matching_block_id=9277410_107323228_0_2_0&amp;sr_pri_blocks=9277410_107323228_0_2_0__151182%2C9277410_107323228_0_2_0__151182%2C9277401_107323228_0_2_0__135342&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>21.651 lei</t>
-  </si>
-  <si>
-    <t>Duplex Sagrada Familia</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/duplex-sagrada-familia.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=21&amp;hapos=21&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=467147602_333927248_0_0_0&amp;highlighted_blocks=467147602_333927248_0_0_0&amp;matching_block_id=467147602_333927248_0_0_0&amp;sr_pri_blocks=467147602_333927248_0_0_0__223780&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>11.069 lei</t>
-  </si>
-  <si>
-    <t>8,1</t>
-  </si>
-  <si>
-    <t>Hostal Portugal</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/pension-portugal.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=22&amp;hapos=22&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=27524208_88206095_0_0_0%2C27524208_88206095_0_0_0%2C27524205_88206095_0_0_0&amp;highlighted_blocks=27524208_88206095_0_0_0%2C27524208_88206095_0_0_0%2C27524205_88206095_0_0_0&amp;matching_block_id=27524208_88206095_0_0_0&amp;sr_pri_blocks=27524208_88206095_0_0_0__42042%2C27524208_88206095_0_0_0__42042%2C27524205_88206095_0_0_0__42042&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>6.239 lei</t>
-  </si>
-  <si>
-    <t>Unique Cozy Scenic Penthouse</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/unique-cozy-scenic-penthouse.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=23&amp;hapos=23&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=198952601_119720213_7_0_0&amp;highlighted_blocks=198952601_119720213_7_0_0&amp;matching_block_id=198952601_119720213_7_0_0&amp;sr_pri_blocks=198952601_119720213_7_0_0__298560&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>14.768 lei</t>
-  </si>
-  <si>
-    <t>la 2,5 km de centru</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/hotelantibesbarcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=24&amp;hapos=24&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=9131901_246265787_0_2_0%2C9131903_246265787_0_2_0%2C9131903_246265787_0_2_0&amp;highlighted_blocks=9131901_246265787_0_2_0%2C9131903_246265787_0_2_0%2C9131903_246265787_0_2_0&amp;matching_block_id=9131901_246265787_0_2_0&amp;sr_pri_blocks=9131901_246265787_0_2_0__81192%2C9131903_246265787_0_2_0__114093%2C9131903_246265787_0_2_0__114093&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>Casa Gracia</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/hostel-casa-gracia.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=25&amp;hapos=25&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506065&amp;all_sr_blocks=25515426_295384839_0_0_0%2C25515426_295384839_0_0_0&amp;highlighted_blocks=25515426_295384839_0_0_0%2C25515426_295384839_0_0_0&amp;matching_block_id=25515426_295384839_0_0_0&amp;sr_pri_blocks=25515426_295384839_0_0_0__176184%2C25515426_295384839_0_0_0__176184&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>17.430 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/apartments-in-barcelona-dames.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=1&amp;hapos=651&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506110&amp;all_sr_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;highlighted_blocks=1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0%2C1322401_95137168_2_0_0&amp;matching_block_id=1322401_95137168_2_0_0&amp;sr_pri_blocks=1322401_95137168_2_0_0__144535%2C1322401_95137168_2_0_0__144535%2C1322401_95137168_2_0_0__144535%2C1322401_95137168_2_0_0__144535&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>28.598 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/classbedroom-ii.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuAK4yd2OBsACAdICJDRmYjNhMjU4LWM1NTAtNDgyZS04MzQ5LWE1MmZmNWU2M2E0ZdgCBuACAQ&amp;sid=54715663d002cdd6654d031b3f7823e5&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=2&amp;hapos=652&amp;sr_order=popularity&amp;srpvid=7ed99a08fea40128&amp;srepoch=1641506110&amp;all_sr_blocks=1876408_335854946_2_0_0%2C1876407_335854946_2_0_0%2C1876405_335854946_2_0_0%2C1876406_335854946_2_0_0&amp;highlighted_blocks=1876408_335854946_2_0_0%2C1876407_335854946_2_0_0%2C1876405_335854946_2_0_0%2C1876406_335854946_2_0_0&amp;matching_block_id=1876408_335854946_2_0_0&amp;sr_pri_blocks=1876408_335854946_2_0_0__105700%2C1876407_335854946_2_0_0__105700%2C1876405_335854946_2_0_0__105700%2C1876406_335854946_2_0_0__105700&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>20.914 lei</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/ca-39-l-mateu.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=1&amp;hapos=1&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=240710701_178269580_0_0_0&amp;highlighted_blocks=240710701_178269580_0_0_0&amp;matching_block_id=240710701_178269580_0_0_0&amp;sr_pri_blocks=240710701_178269580_0_0_0__317640&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/peninsular-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=2&amp;hapos=2&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=38860901_266040762_0_1_0%2C38860902_266040762_0_1_0%2C38860903_266040762_0_1_0&amp;highlighted_blocks=38860901_266040762_0_1_0%2C38860902_266040762_0_1_0%2C38860903_266040762_0_1_0&amp;matching_block_id=38860901_266040762_0_1_0&amp;sr_pri_blocks=38860901_266040762_0_1_0__62121%2C38860902_266040762_0_1_0__93042%2C38860903_266040762_0_1_0__120363&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/hostalin-barcelona.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=3&amp;hapos=3&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=39007205_298407854_0_0_0%2C39007205_298407854_0_0_0%2C39007205_298407854_0_0_0&amp;highlighted_blocks=39007205_298407854_0_0_0%2C39007205_298407854_0_0_0%2C39007205_298407854_0_0_0&amp;matching_block_id=39007205_298407854_0_0_0&amp;sr_pri_blocks=39007205_298407854_0_0_0__60942%2C39007205_298407854_0_0_0__60942%2C39007205_298407854_0_0_0__60942&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/poolhouses-lila-house.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=4&amp;hapos=4&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=250494701_188944878_10_0_0&amp;highlighted_blocks=250494701_188944878_10_0_0&amp;matching_block_id=250494701_188944878_10_0_0&amp;sr_pri_blocks=250494701_188944878_10_0_0__475552&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/hostal-orleans.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=5&amp;hapos=5&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=38790506_298815720_0_0_0%2C38790504_298815720_0_0_0%2C38790505_298815720_0_0_0&amp;highlighted_blocks=38790506_298815720_0_0_0%2C38790504_298815720_0_0_0%2C38790505_298815720_0_0_0&amp;matching_block_id=38790506_298815720_0_0_0&amp;sr_pri_blocks=38790506_298815720_0_0_0__173739%2C38790504_298815720_0_0_0__105748%2C38790505_298815720_0_0_0__62541&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/luxury-seaview-forum-ccib-apartment.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=6&amp;hapos=6&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=654142101_272395774_8_0_0&amp;highlighted_blocks=654142101_272395774_8_0_0&amp;matching_block_id=654142101_272395774_8_0_0&amp;sr_pri_blocks=654142101_272395774_8_0_0__305440&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/big-charming-3-bedroom-apt-in-heart-of-bcn.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=7&amp;hapos=7&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=555968401_206692934_0_0_0&amp;highlighted_blocks=555968401_206692934_0_0_0&amp;matching_block_id=555968401_206692934_0_0_0&amp;sr_pri_blocks=555968401_206692934_0_0_0__232440&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/pereiv.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=8&amp;hapos=8&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=9094311_331231580_0_0_0%2C9094312_331231580_0_0_0%2C9094312_331231580_0_0_0&amp;highlighted_blocks=9094311_331231580_0_0_0%2C9094312_331231580_0_0_0%2C9094312_331231580_0_0_0&amp;matching_block_id=9094311_331231580_0_0_0&amp;sr_pri_blocks=9094311_331231580_0_0_0__105760%2C9094312_331231580_0_0_0__140820%2C9094312_331231580_0_0_0__140820&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/sagrada-familia-apartment-barcelona5.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=9&amp;hapos=9&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=159140401_262866637_8_0_0&amp;highlighted_blocks=159140401_262866637_8_0_0&amp;matching_block_id=159140401_262866637_8_0_0&amp;sr_pri_blocks=159140401_262866637_8_0_0__199060&amp;from=searchresults#hotelTmpl</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/hotel/es/apartment-guell.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALqzt2OBsACAdICJGIwYzQxNjNlLTQ2MmQtNDg5My05OWNiLTRiNTE1ZTYwZjAyMtgCBuACAQ&amp;sid=92debfa9aba7473276868e091ec30ef1&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=10&amp;hapos=10&amp;sr_order=popularity&amp;srpvid=7be89b72a9f3000b&amp;srepoch=1641506789&amp;all_sr_blocks=128512201_86982088_0_0_0&amp;highlighted_blocks=128512201_86982088_0_0_0&amp;matching_block_id=128512201_86982088_0_0_0&amp;sr_pri_blocks=128512201_86982088_0_0_0__251138&amp;from=searchresults#hotelTmpl</t>
+    <t>https://www.booking.com/hotel/es/amplio-y-bien-situado-para-10-personas.ro.html?label=gen173nr-1FCAEoggI46AdIM1gEaMABiAEBmAEguAEXyAEM2AEB6AEB-AELiAIBqAIDuALa0-WOBsACAdICJGJhZTg2Njc4LTMzNTctNGZkNC1hMDJkLTFjNGEwNGE4ZjFlNdgCBuACAQ&amp;sid=38a3daac23f900bb062898cea50b226e&amp;aid=304142&amp;ucfs=1&amp;arphpl=1&amp;checkin=2022-11-28&amp;checkout=2022-12-10&amp;dest_id=-372490&amp;dest_type=city&amp;group_adults=5&amp;req_adults=5&amp;no_rooms=3&amp;group_children=3&amp;req_children=3&amp;age=12&amp;req_age=12&amp;age=2&amp;req_age=2&amp;age=3&amp;req_age=3&amp;hpos=10&amp;hapos=10&amp;sr_order=popularity&amp;srpvid=bb284b0b4d330042&amp;srepoch=1641638423&amp;all_sr_blocks=77877104_326137462_0_0_0&amp;highlighted_blocks=77877104_326137462_0_0_0&amp;matching_block_id=77877104_326137462_0_0_0&amp;sr_pri_blocks=77877104_326137462_0_0_0__293440&amp;from=searchresults#hotelTmpl</t>
+  </si>
+  <si>
+    <t>14.509 lei</t>
   </si>
 </sst>
 </file>
@@ -969,180 +960,183 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>180</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>190</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1150,33 +1144,33 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -1184,64 +1178,64 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -1252,30 +1246,30 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -1283,50 +1277,50 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1334,67 +1328,67 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1402,16 +1396,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -1419,33 +1413,33 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1453,27 +1447,27 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -1484,47 +1478,47 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
         <v>26</v>
       </c>
-      <c r="B34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" t="s">
-        <v>27</v>
-      </c>
       <c r="E34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
@@ -1532,33 +1526,33 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
         <v>28</v>
-      </c>
-      <c r="B36" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
@@ -1566,27 +1560,27 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -1597,16 +1591,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
@@ -1614,13 +1608,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
         <v>9</v>
@@ -1628,16 +1622,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E42" t="s">
         <v>14</v>
@@ -1645,44 +1639,44 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" t="s">
         <v>28</v>
-      </c>
-      <c r="B43" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -1693,30 +1687,30 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1727,16 +1721,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E48" t="s">
         <v>9</v>
@@ -1744,33 +1738,33 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D49" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -1778,16 +1772,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>

</xml_diff>